<commit_message>
VCF SCG 901-20260107-01 & 803-20260107-01
</commit_message>
<xml_diff>
--- a/security-configuration-hardening-guide/vsan/8.0/vmware-vsphere-security-configuration-guide-8-controls.xlsx
+++ b/security-configuration-hardening-guide/vsan/8.0/vmware-vsphere-security-configuration-guide-8-controls.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB5A40B-F560-465B-8791-9BF7671F79CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3F1D88-3A1F-496D-BD42-B1613BB85D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="61656" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="18" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3705" uniqueCount="1272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3705" uniqueCount="1276">
   <si>
     <t>See the included documentation for important guidance and instructions.</t>
   </si>
@@ -4416,10 +4416,22 @@
     <t>This guidance evolves. Please check the current revision at: https://github.com/vmware/vcf-security-and-compliance-guidelines</t>
   </si>
   <si>
-    <t>Version 803-20250904-01</t>
-  </si>
-  <si>
     <t>It is important to ensure that sufficient information is present in audit logs for diagnostics and forensics purposes. The recommendation for this parameter in the Security Configuration Guide has traditionally been "info" but with the introduction of the audit logging subsystems there is no longer a need for the extra log traffic. As such, the recommendation has changed to use the product default of "error" unless debugging or troubleshooting.</t>
+  </si>
+  <si>
+    <t>Version 803-20260107-01</t>
+  </si>
+  <si>
+    <t>(Get-CisService -Name "com.vmware.appliance.local_accounts.policy").get() | Select-Object -ExpandProperty max_days</t>
+  </si>
+  <si>
+    <t>(Get-CisService -Name "com.vmware.appliance.local_accounts.policy").set(@{max_days=-1})</t>
+  </si>
+  <si>
+    <t>(Get-CisService -Name "com.vmware.appliance.recovery.backup.schedules").list()</t>
+  </si>
+  <si>
+    <t>(Get-CisService -Name "com.vmware.appliance.networking.firewall.inbound").get()</t>
   </si>
 </sst>
 </file>
@@ -7466,49 +7478,49 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="38.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="181.109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="159.109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="38.109375" style="6"/>
+    <col min="1" max="1" width="181.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="159.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="38.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1268</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>1270</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="26"/>
     </row>
-    <row r="5" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>1269</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="26"/>
     </row>
-    <row r="7" spans="1:1" ht="110.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>1220</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="59"/>
     </row>
-    <row r="9" spans="1:1" ht="273" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" ht="273" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>1264</v>
       </c>
@@ -7529,23 +7541,23 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="38.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.44140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="159.109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="38.109375" style="6"/>
+    <col min="1" max="1" width="55.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="159.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="38.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="17" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="17" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1265</v>
       </c>
       <c r="B1" s="25"/>
     </row>
-    <row r="2" spans="1:8" s="17" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="17" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -7555,12 +7567,12 @@
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
     </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -7568,7 +7580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>341</v>
       </c>
@@ -7577,7 +7589,7 @@
       </c>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>613</v>
       </c>
@@ -7586,7 +7598,7 @@
       </c>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>895</v>
       </c>
@@ -7595,7 +7607,7 @@
       </c>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>1258</v>
       </c>
@@ -7604,7 +7616,7 @@
       </c>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>1257</v>
       </c>
@@ -7613,7 +7625,7 @@
       </c>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>1259</v>
       </c>
@@ -7622,7 +7634,7 @@
       </c>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:8" ht="234" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
@@ -7631,7 +7643,7 @@
       </c>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>496</v>
       </c>
@@ -7640,7 +7652,7 @@
       </c>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
@@ -7649,7 +7661,7 @@
       </c>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -7658,7 +7670,7 @@
       </c>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>82</v>
       </c>
@@ -7667,7 +7679,7 @@
       </c>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>486</v>
       </c>
@@ -7676,7 +7688,7 @@
       </c>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>342</v>
       </c>
@@ -7685,7 +7697,7 @@
       </c>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
@@ -7694,7 +7706,7 @@
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
@@ -7703,7 +7715,7 @@
       </c>
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>778</v>
       </c>
@@ -7712,7 +7724,7 @@
       </c>
       <c r="C20" s="6"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>12</v>
       </c>
@@ -7721,7 +7733,7 @@
       </c>
       <c r="C21" s="6"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
@@ -7730,7 +7742,7 @@
       </c>
       <c r="C22" s="6"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>994</v>
       </c>
@@ -7739,7 +7751,7 @@
       </c>
       <c r="C23" s="6"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>1242</v>
       </c>
@@ -7748,7 +7760,7 @@
       </c>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>1186</v>
       </c>
@@ -7757,7 +7769,7 @@
       </c>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>1142</v>
       </c>
@@ -7766,7 +7778,7 @@
       </c>
       <c r="C26" s="6"/>
     </row>
-    <row r="27" spans="1:3" ht="140.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>1167</v>
       </c>
@@ -7775,7 +7787,7 @@
       </c>
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>1187</v>
       </c>
@@ -7784,7 +7796,7 @@
       </c>
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>1141</v>
       </c>
@@ -7793,7 +7805,7 @@
       </c>
       <c r="C29" s="6"/>
     </row>
-    <row r="30" spans="1:3" ht="140.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>1168</v>
       </c>
@@ -7802,7 +7814,7 @@
       </c>
       <c r="C30" s="6"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>920</v>
       </c>
@@ -7830,15 +7842,15 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="38.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="14" customWidth="1"/>
-    <col min="3" max="4" width="85.6640625" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="38.109375" style="6"/>
+    <col min="1" max="1" width="60.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="14" customWidth="1"/>
+    <col min="3" max="4" width="85.7109375" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="38.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1266</v>
       </c>
@@ -7846,20 +7858,20 @@
       <c r="C1" s="25"/>
       <c r="D1" s="24"/>
     </row>
-    <row r="2" spans="1:4" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
       <c r="D2" s="23"/>
     </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="19"/>
       <c r="C3" s="18"/>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>341</v>
       </c>
@@ -7873,7 +7885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="8" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="8" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>17</v>
       </c>
@@ -7887,7 +7899,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="8" customFormat="1" ht="202.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" s="8" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>1044</v>
       </c>
@@ -7901,7 +7913,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="8" customFormat="1" ht="156" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" s="8" customFormat="1" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>18</v>
       </c>
@@ -7915,7 +7927,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="8" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" s="8" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>19</v>
       </c>
@@ -7929,7 +7941,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="8" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>20</v>
       </c>
@@ -7943,7 +7955,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="8" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" s="8" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
@@ -7957,7 +7969,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="8" customFormat="1" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" s="8" customFormat="1" ht="378" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>22</v>
       </c>
@@ -7971,7 +7983,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="8" customFormat="1" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" s="8" customFormat="1" ht="378" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>336</v>
       </c>
@@ -7985,7 +7997,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="8" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" s="8" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>1038</v>
       </c>
@@ -7999,7 +8011,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="8" customFormat="1" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" s="8" customFormat="1" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -8013,7 +8025,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="8" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>26</v>
       </c>
@@ -8027,7 +8039,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="8" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" s="8" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>27</v>
       </c>
@@ -8041,7 +8053,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="8" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" s="8" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>1206</v>
       </c>
@@ -8055,7 +8067,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="8" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" s="8" customFormat="1" ht="189" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>644</v>
       </c>
@@ -8069,7 +8081,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="8" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>614</v>
       </c>
@@ -8083,7 +8095,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="8" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>28</v>
       </c>
@@ -8097,7 +8109,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="8" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" s="8" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>25</v>
       </c>
@@ -8111,7 +8123,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="8" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" s="8" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>24</v>
       </c>
@@ -8125,7 +8137,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="8" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" s="8" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>333</v>
       </c>
@@ -8139,13 +8151,13 @@
         <v>335</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
     </row>
   </sheetData>
@@ -8168,18 +8180,18 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="38.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="14" customWidth="1"/>
-    <col min="3" max="4" width="85.6640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="55.6640625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="200.6640625" style="14" customWidth="1"/>
-    <col min="8" max="16384" width="38.109375" style="6"/>
+    <col min="1" max="1" width="60.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="14" customWidth="1"/>
+    <col min="3" max="4" width="85.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="55.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="200.7109375" style="14" customWidth="1"/>
+    <col min="8" max="16384" width="38.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>1267</v>
       </c>
@@ -8188,22 +8200,22 @@
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:7" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
     </row>
-    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="19"/>
       <c r="C3" s="18"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>341</v>
       </c>
@@ -8226,7 +8238,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>67</v>
       </c>
@@ -8249,7 +8261,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>73</v>
       </c>
@@ -8272,7 +8284,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -8295,7 +8307,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>47</v>
       </c>
@@ -8318,7 +8330,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="202.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>78</v>
       </c>
@@ -8341,7 +8353,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
@@ -8364,7 +8376,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>43</v>
       </c>
@@ -8387,7 +8399,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>59</v>
       </c>
@@ -8410,7 +8422,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>63</v>
       </c>
@@ -8433,7 +8445,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="312" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="315" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>51</v>
       </c>
@@ -8456,7 +8468,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>55</v>
       </c>
@@ -8494,39 +8506,39 @@
   <dimension ref="A1:AH160"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+      <selection activeCell="A127" sqref="A127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="38.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="100.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" style="22" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="22" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="22" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="24.109375" style="22" customWidth="1"/>
-    <col min="7" max="7" width="30.6640625" style="22" customWidth="1"/>
-    <col min="8" max="8" width="116.109375" style="21" customWidth="1"/>
-    <col min="9" max="9" width="148.5546875" style="22" customWidth="1"/>
-    <col min="10" max="10" width="70.33203125" style="22" customWidth="1"/>
-    <col min="11" max="12" width="34.5546875" style="22" customWidth="1"/>
-    <col min="13" max="13" width="19.6640625" style="21" customWidth="1"/>
-    <col min="14" max="14" width="23.6640625" style="22" customWidth="1"/>
-    <col min="15" max="15" width="32.6640625" style="22" customWidth="1"/>
-    <col min="16" max="16" width="68.44140625" style="21" customWidth="1"/>
-    <col min="17" max="17" width="196.109375" style="28" customWidth="1"/>
-    <col min="18" max="18" width="200.5546875" style="22" customWidth="1"/>
-    <col min="19" max="20" width="30.88671875" style="22" customWidth="1"/>
-    <col min="21" max="21" width="19.44140625" style="22" customWidth="1"/>
-    <col min="22" max="26" width="32.109375" style="22" customWidth="1"/>
-    <col min="27" max="27" width="20.88671875" style="22" customWidth="1"/>
-    <col min="28" max="30" width="30.6640625" style="22" customWidth="1"/>
-    <col min="31" max="31" width="57.44140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.6640625" style="22" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="38.109375" style="21"/>
+    <col min="1" max="1" width="100.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="22" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="22" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" style="22" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" style="22" customWidth="1"/>
+    <col min="8" max="8" width="116.140625" style="21" customWidth="1"/>
+    <col min="9" max="9" width="148.5703125" style="22" customWidth="1"/>
+    <col min="10" max="10" width="70.28515625" style="22" customWidth="1"/>
+    <col min="11" max="12" width="34.5703125" style="22" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" style="21" customWidth="1"/>
+    <col min="14" max="14" width="23.7109375" style="22" customWidth="1"/>
+    <col min="15" max="15" width="32.7109375" style="22" customWidth="1"/>
+    <col min="16" max="16" width="68.42578125" style="21" customWidth="1"/>
+    <col min="17" max="17" width="196.140625" style="28" customWidth="1"/>
+    <col min="18" max="18" width="200.5703125" style="22" customWidth="1"/>
+    <col min="19" max="20" width="30.85546875" style="22" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" style="22" customWidth="1"/>
+    <col min="22" max="26" width="32.140625" style="22" customWidth="1"/>
+    <col min="27" max="27" width="20.85546875" style="22" customWidth="1"/>
+    <col min="28" max="30" width="30.7109375" style="22" customWidth="1"/>
+    <col min="31" max="31" width="57.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="33" max="16384" width="38.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>473</v>
       </c>
@@ -8549,9 +8561,9 @@
       <c r="AE1" s="21"/>
       <c r="AF1" s="21"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -8572,7 +8584,7 @@
       <c r="AE2" s="21"/>
       <c r="AF2" s="21"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="Q3" s="22"/>
       <c r="AB3" s="21"/>
       <c r="AC3" s="21"/>
@@ -8580,7 +8592,7 @@
       <c r="AE3" s="21"/>
       <c r="AF3" s="21"/>
     </row>
-    <row r="4" spans="1:32" s="2" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>341</v>
       </c>
@@ -8663,7 +8675,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="5" spans="1:32" s="52" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" s="52" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>154</v>
       </c>
@@ -8747,7 +8759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:32" s="52" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" s="52" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>529</v>
       </c>
@@ -8830,7 +8842,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:32" s="7" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" s="7" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>157</v>
       </c>
@@ -8914,7 +8926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:32" s="7" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" s="7" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>160</v>
       </c>
@@ -8998,7 +9010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:32" s="7" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" s="7" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>163</v>
       </c>
@@ -9082,7 +9094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:32" s="7" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" s="7" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>92</v>
       </c>
@@ -9167,7 +9179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:32" s="5" customFormat="1" ht="202.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" s="5" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>530</v>
       </c>
@@ -9250,7 +9262,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:32" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>913</v>
       </c>
@@ -9333,7 +9345,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:32" s="5" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" s="5" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>83</v>
       </c>
@@ -9416,7 +9428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:32" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>595</v>
       </c>
@@ -9436,7 +9448,7 @@
         <v>612</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>153</v>
+        <v>68</v>
       </c>
       <c r="H14" s="31" t="s">
         <v>511</v>
@@ -9451,13 +9463,13 @@
         <v>30</v>
       </c>
       <c r="L14" s="33">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="M14" s="32" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="N14" s="32" t="s">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="O14" s="33" t="s">
         <v>87</v>
@@ -9471,7 +9483,7 @@
       </c>
       <c r="R14" s="34" t="str">
         <f>"Get-VMHost -Name $ESXi | Get-AdvancedSetting "&amp;Table252329[[#This Row],[Configuration Parameter]]&amp;" | Set-AdvancedSetting -Value "&amp;Table252329[[#This Row],[Baseline Suggested Value]]</f>
-        <v>Get-VMHost -Name $ESXi | Get-AdvancedSetting Config.HostAgent.vmacore.soap.sessionTimeout | Set-AdvancedSetting -Value 30</v>
+        <v>Get-VMHost -Name $ESXi | Get-AdvancedSetting Config.HostAgent.vmacore.soap.sessionTimeout | Set-AdvancedSetting -Value 10</v>
       </c>
       <c r="S14" s="33" t="b">
         <v>1</v>
@@ -9501,7 +9513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:32" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
         <v>166</v>
       </c>
@@ -9586,7 +9598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:32" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>168</v>
       </c>
@@ -9671,7 +9683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:27" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>465</v>
       </c>
@@ -9754,7 +9766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:27" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>466</v>
       </c>
@@ -9839,7 +9851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:27" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>789</v>
       </c>
@@ -9922,7 +9934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:27" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>467</v>
       </c>
@@ -10005,7 +10017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:27" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>468</v>
       </c>
@@ -10088,7 +10100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:27" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>469</v>
       </c>
@@ -10171,7 +10183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:27" s="5" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" s="5" customFormat="1" ht="126" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
         <v>597</v>
       </c>
@@ -10254,7 +10266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:27" s="5" customFormat="1" ht="405.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" s="5" customFormat="1" ht="393.75" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>91</v>
       </c>
@@ -10337,7 +10349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:27" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>510</v>
       </c>
@@ -10420,7 +10432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:27" s="5" customFormat="1" ht="358.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" s="5" customFormat="1" ht="362.25" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>132</v>
       </c>
@@ -10503,7 +10515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:27" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
         <v>186</v>
       </c>
@@ -10588,7 +10600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:27" s="5" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
         <v>599</v>
       </c>
@@ -10673,7 +10685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:27" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
         <v>343</v>
       </c>
@@ -10756,7 +10768,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="30" spans="1:27" s="5" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" s="5" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>1037</v>
       </c>
@@ -10839,7 +10851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:27" s="5" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>96</v>
       </c>
@@ -10924,7 +10936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:27" s="5" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>100</v>
       </c>
@@ -11007,7 +11019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:27" s="5" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:27" s="5" customFormat="1" ht="189" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
         <v>105</v>
       </c>
@@ -11090,7 +11102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:27" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:27" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
         <v>586</v>
       </c>
@@ -11175,7 +11187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:27" s="5" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:27" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
         <v>589</v>
       </c>
@@ -11260,7 +11272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:27" s="5" customFormat="1" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:27" s="5" customFormat="1" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>587</v>
       </c>
@@ -11343,7 +11355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:27" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:27" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>585</v>
       </c>
@@ -11428,7 +11440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:27" s="5" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:27" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>590</v>
       </c>
@@ -11511,7 +11523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:27" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:27" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
         <v>170</v>
       </c>
@@ -11596,7 +11608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:27" s="5" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:27" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
         <v>591</v>
       </c>
@@ -11622,7 +11634,7 @@
         <v>574</v>
       </c>
       <c r="I40" s="60" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="J40" s="32" t="s">
         <v>444</v>
@@ -11681,7 +11693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:27" s="29" customFormat="1" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:27" s="29" customFormat="1" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
         <v>108</v>
       </c>
@@ -11764,7 +11776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:27" s="29" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:27" s="29" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
         <v>110</v>
       </c>
@@ -11848,7 +11860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:27" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:27" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
         <v>588</v>
       </c>
@@ -11933,7 +11945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:27" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:27" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
         <v>598</v>
       </c>
@@ -12018,7 +12030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:27" s="5" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:27" s="5" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
         <v>432</v>
       </c>
@@ -12103,7 +12115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:27" s="5" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:27" s="5" customFormat="1" ht="126" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
         <v>175</v>
       </c>
@@ -12188,7 +12200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:27" s="5" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:27" s="5" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A47" s="39" t="s">
         <v>307</v>
       </c>
@@ -12273,7 +12285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:27" s="5" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:27" s="5" customFormat="1" ht="126" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
         <v>137</v>
       </c>
@@ -12356,7 +12368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:28" s="5" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28" s="5" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
         <v>140</v>
       </c>
@@ -12439,7 +12451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:28" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
         <v>141</v>
       </c>
@@ -12522,7 +12534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:28" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A51" s="31" t="s">
         <v>594</v>
       </c>
@@ -12605,7 +12617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:28" s="5" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:28" s="5" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A52" s="31" t="s">
         <v>593</v>
       </c>
@@ -12688,7 +12700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:28" s="5" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:28" s="5" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A53" s="31" t="s">
         <v>1233</v>
       </c>
@@ -12771,7 +12783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:28" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:28" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="s">
         <v>144</v>
       </c>
@@ -12856,7 +12868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:28" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:28" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A55" s="31" t="s">
         <v>177</v>
       </c>
@@ -12941,7 +12953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:28" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:28" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A56" s="31" t="s">
         <v>180</v>
       </c>
@@ -13026,7 +13038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:28" s="5" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:28" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A57" s="31" t="s">
         <v>592</v>
       </c>
@@ -13109,7 +13121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:28" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:28" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A58" s="31" t="s">
         <v>983</v>
       </c>
@@ -13192,7 +13204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:28" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:28" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A59" s="31" t="s">
         <v>955</v>
       </c>
@@ -13275,7 +13287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:28" s="7" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:28" s="7" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A60" s="31" t="s">
         <v>953</v>
       </c>
@@ -13358,7 +13370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:28" s="7" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:28" s="7" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A61" s="31" t="s">
         <v>957</v>
       </c>
@@ -13441,7 +13453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:28" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A62" s="31" t="s">
         <v>958</v>
       </c>
@@ -13525,7 +13537,7 @@
       </c>
       <c r="AB62" s="15"/>
     </row>
-    <row r="63" spans="1:28" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A63" s="31" t="s">
         <v>952</v>
       </c>
@@ -13609,7 +13621,7 @@
       </c>
       <c r="AB63" s="15"/>
     </row>
-    <row r="64" spans="1:28" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:28" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A64" s="31" t="s">
         <v>951</v>
       </c>
@@ -13693,7 +13705,7 @@
       </c>
       <c r="AB64" s="15"/>
     </row>
-    <row r="65" spans="1:34" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:34" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A65" s="31" t="s">
         <v>967</v>
       </c>
@@ -13777,7 +13789,7 @@
       </c>
       <c r="AB65" s="15"/>
     </row>
-    <row r="66" spans="1:34" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:34" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A66" s="31" t="s">
         <v>959</v>
       </c>
@@ -13861,7 +13873,7 @@
       </c>
       <c r="AB66" s="15"/>
     </row>
-    <row r="67" spans="1:34" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:34" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A67" s="31" t="s">
         <v>956</v>
       </c>
@@ -13945,7 +13957,7 @@
       </c>
       <c r="AB67" s="15"/>
     </row>
-    <row r="68" spans="1:34" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:34" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A68" s="31" t="s">
         <v>954</v>
       </c>
@@ -14029,7 +14041,7 @@
       </c>
       <c r="AB68" s="15"/>
     </row>
-    <row r="69" spans="1:34" s="5" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:34" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A69" s="31" t="s">
         <v>112</v>
       </c>
@@ -14113,7 +14125,7 @@
       </c>
       <c r="AB69" s="15"/>
     </row>
-    <row r="70" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A70" s="31" t="s">
         <v>922</v>
       </c>
@@ -14197,7 +14209,7 @@
       </c>
       <c r="AB70" s="15"/>
     </row>
-    <row r="71" spans="1:34" s="5" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:34" s="5" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A71" s="31" t="s">
         <v>518</v>
       </c>
@@ -14281,7 +14293,7 @@
       </c>
       <c r="AB71" s="15"/>
     </row>
-    <row r="72" spans="1:34" s="5" customFormat="1" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:34" s="5" customFormat="1" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A72" s="31" t="s">
         <v>1036</v>
       </c>
@@ -14365,7 +14377,7 @@
       </c>
       <c r="AB72" s="15"/>
     </row>
-    <row r="73" spans="1:34" s="5" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:34" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A73" s="39" t="s">
         <v>308</v>
       </c>
@@ -14451,7 +14463,7 @@
       </c>
       <c r="AB73" s="15"/>
     </row>
-    <row r="74" spans="1:34" s="5" customFormat="1" ht="202.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:34" s="5" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A74" s="31" t="s">
         <v>596</v>
       </c>
@@ -14535,7 +14547,7 @@
       </c>
       <c r="AB74" s="15"/>
     </row>
-    <row r="75" spans="1:34" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:34" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A75" s="31" t="s">
         <v>184</v>
       </c>
@@ -14621,7 +14633,7 @@
       </c>
       <c r="AB75" s="15"/>
     </row>
-    <row r="76" spans="1:34" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:34" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A76" s="31" t="s">
         <v>119</v>
       </c>
@@ -14705,7 +14717,7 @@
       </c>
       <c r="AB76" s="15"/>
     </row>
-    <row r="77" spans="1:34" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:34" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A77" s="31" t="s">
         <v>150</v>
       </c>
@@ -14789,7 +14801,7 @@
       </c>
       <c r="AB77" s="15"/>
     </row>
-    <row r="78" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A78" s="31" t="s">
         <v>120</v>
       </c>
@@ -14874,7 +14886,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="79" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A79" s="31" t="s">
         <v>123</v>
       </c>
@@ -14957,7 +14969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:34" s="5" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:34" s="5" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A80" s="31" t="s">
         <v>288</v>
       </c>
@@ -15047,7 +15059,7 @@
       <c r="AG80" s="15"/>
       <c r="AH80" s="15"/>
     </row>
-    <row r="81" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A81" s="31" t="s">
         <v>821</v>
       </c>
@@ -15137,7 +15149,7 @@
       <c r="AG81" s="15"/>
       <c r="AH81" s="15"/>
     </row>
-    <row r="82" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A82" s="31" t="s">
         <v>824</v>
       </c>
@@ -15227,7 +15239,7 @@
       <c r="AG82" s="15"/>
       <c r="AH82" s="15"/>
     </row>
-    <row r="83" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A83" s="34" t="s">
         <v>749</v>
       </c>
@@ -15317,7 +15329,7 @@
       <c r="AG83" s="15"/>
       <c r="AH83" s="15"/>
     </row>
-    <row r="84" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A84" s="31" t="s">
         <v>746</v>
       </c>
@@ -15407,7 +15419,7 @@
       <c r="AG84" s="15"/>
       <c r="AH84" s="15"/>
     </row>
-    <row r="85" spans="1:34" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:34" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A85" s="31" t="s">
         <v>748</v>
       </c>
@@ -15497,7 +15509,7 @@
       <c r="AG85" s="15"/>
       <c r="AH85" s="15"/>
     </row>
-    <row r="86" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A86" s="31" t="s">
         <v>747</v>
       </c>
@@ -15587,7 +15599,7 @@
       <c r="AG86" s="15"/>
       <c r="AH86" s="15"/>
     </row>
-    <row r="87" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A87" s="31" t="s">
         <v>745</v>
       </c>
@@ -15677,7 +15689,7 @@
       <c r="AG87" s="15"/>
       <c r="AH87" s="15"/>
     </row>
-    <row r="88" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A88" s="31" t="s">
         <v>830</v>
       </c>
@@ -15767,7 +15779,7 @@
       <c r="AG88" s="15"/>
       <c r="AH88" s="15"/>
     </row>
-    <row r="89" spans="1:34" s="5" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:34" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A89" s="31" t="s">
         <v>904</v>
       </c>
@@ -15857,7 +15869,7 @@
       <c r="AG89" s="15"/>
       <c r="AH89" s="15"/>
     </row>
-    <row r="90" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A90" s="31" t="s">
         <v>835</v>
       </c>
@@ -15947,7 +15959,7 @@
       <c r="AG90" s="15"/>
       <c r="AH90" s="15"/>
     </row>
-    <row r="91" spans="1:34" s="5" customFormat="1" ht="156" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:34" s="5" customFormat="1" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A91" s="31" t="s">
         <v>303</v>
       </c>
@@ -16037,7 +16049,7 @@
       <c r="AG91" s="15"/>
       <c r="AH91" s="15"/>
     </row>
-    <row r="92" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A92" s="31" t="s">
         <v>822</v>
       </c>
@@ -16127,7 +16139,7 @@
       <c r="AG92" s="15"/>
       <c r="AH92" s="15"/>
     </row>
-    <row r="93" spans="1:34" s="5" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:34" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A93" s="31" t="s">
         <v>292</v>
       </c>
@@ -16217,7 +16229,7 @@
       <c r="AG93" s="15"/>
       <c r="AH93" s="15"/>
     </row>
-    <row r="94" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A94" s="31" t="s">
         <v>820</v>
       </c>
@@ -16307,7 +16319,7 @@
       <c r="AG94" s="15"/>
       <c r="AH94" s="15"/>
     </row>
-    <row r="95" spans="1:34" s="5" customFormat="1" ht="156" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:34" s="5" customFormat="1" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A95" s="31" t="s">
         <v>299</v>
       </c>
@@ -16397,7 +16409,7 @@
       <c r="AG95" s="15"/>
       <c r="AH95" s="15"/>
     </row>
-    <row r="96" spans="1:34" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:34" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="31" t="s">
         <v>268</v>
       </c>
@@ -16487,7 +16499,7 @@
       <c r="AG96" s="15"/>
       <c r="AH96" s="15"/>
     </row>
-    <row r="97" spans="1:34" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:34" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="31" t="s">
         <v>763</v>
       </c>
@@ -16577,7 +16589,7 @@
       <c r="AG97" s="15"/>
       <c r="AH97" s="15"/>
     </row>
-    <row r="98" spans="1:34" s="5" customFormat="1" ht="405.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:34" s="5" customFormat="1" ht="393.75" x14ac:dyDescent="0.25">
       <c r="A98" s="31" t="s">
         <v>266</v>
       </c>
@@ -16667,7 +16679,7 @@
       <c r="AG98" s="15"/>
       <c r="AH98" s="15"/>
     </row>
-    <row r="99" spans="1:34" s="5" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:34" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A99" s="31" t="s">
         <v>261</v>
       </c>
@@ -16757,7 +16769,7 @@
       <c r="AG99" s="15"/>
       <c r="AH99" s="15"/>
     </row>
-    <row r="100" spans="1:34" s="5" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:34" s="5" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A100" s="31" t="s">
         <v>263</v>
       </c>
@@ -16847,7 +16859,7 @@
       <c r="AG100" s="15"/>
       <c r="AH100" s="15"/>
     </row>
-    <row r="101" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A101" s="31" t="s">
         <v>260</v>
       </c>
@@ -16937,7 +16949,7 @@
       <c r="AG101" s="15"/>
       <c r="AH101" s="15"/>
     </row>
-    <row r="102" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A102" s="39" t="s">
         <v>252</v>
       </c>
@@ -17027,7 +17039,7 @@
       <c r="AG102" s="15"/>
       <c r="AH102" s="15"/>
     </row>
-    <row r="103" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A103" s="39" t="s">
         <v>253</v>
       </c>
@@ -17117,7 +17129,7 @@
       <c r="AG103" s="15"/>
       <c r="AH103" s="15"/>
     </row>
-    <row r="104" spans="1:34" s="5" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:34" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A104" s="31" t="s">
         <v>256</v>
       </c>
@@ -17207,7 +17219,7 @@
       <c r="AG104" s="15"/>
       <c r="AH104" s="15"/>
     </row>
-    <row r="105" spans="1:34" s="5" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:34" s="5" customFormat="1" ht="126" x14ac:dyDescent="0.25">
       <c r="A105" s="39" t="s">
         <v>254</v>
       </c>
@@ -17297,7 +17309,7 @@
       <c r="AG105" s="15"/>
       <c r="AH105" s="15"/>
     </row>
-    <row r="106" spans="1:34" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:34" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="31" t="s">
         <v>258</v>
       </c>
@@ -17387,7 +17399,7 @@
       <c r="AG106" s="15"/>
       <c r="AH106" s="15"/>
     </row>
-    <row r="107" spans="1:34" s="5" customFormat="1" ht="405.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:34" s="5" customFormat="1" ht="393.75" x14ac:dyDescent="0.25">
       <c r="A107" s="31" t="s">
         <v>921</v>
       </c>
@@ -17478,7 +17490,7 @@
       <c r="AG107" s="15"/>
       <c r="AH107" s="15"/>
     </row>
-    <row r="108" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A108" s="31" t="s">
         <v>759</v>
       </c>
@@ -17568,7 +17580,7 @@
       <c r="AG108" s="15"/>
       <c r="AH108" s="15"/>
     </row>
-    <row r="109" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A109" s="31" t="s">
         <v>760</v>
       </c>
@@ -17660,7 +17672,7 @@
       <c r="AG109" s="15"/>
       <c r="AH109" s="15"/>
     </row>
-    <row r="110" spans="1:34" s="5" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:34" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A110" s="31" t="s">
         <v>761</v>
       </c>
@@ -17750,7 +17762,7 @@
       <c r="AG110" s="15"/>
       <c r="AH110" s="15"/>
     </row>
-    <row r="111" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A111" s="31" t="s">
         <v>764</v>
       </c>
@@ -17842,7 +17854,7 @@
       <c r="AG111" s="15"/>
       <c r="AH111" s="15"/>
     </row>
-    <row r="112" spans="1:34" s="5" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:34" s="5" customFormat="1" ht="126" x14ac:dyDescent="0.25">
       <c r="A112" s="31" t="s">
         <v>1132</v>
       </c>
@@ -17932,7 +17944,7 @@
       <c r="AG112" s="15"/>
       <c r="AH112" s="15"/>
     </row>
-    <row r="113" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A113" s="31" t="s">
         <v>272</v>
       </c>
@@ -18022,7 +18034,7 @@
       <c r="AG113" s="15"/>
       <c r="AH113" s="15"/>
     </row>
-    <row r="114" spans="1:34" s="5" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:34" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A114" s="31" t="s">
         <v>273</v>
       </c>
@@ -18112,7 +18124,7 @@
       <c r="AG114" s="15"/>
       <c r="AH114" s="15"/>
     </row>
-    <row r="115" spans="1:34" s="5" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:34" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A115" s="31" t="s">
         <v>274</v>
       </c>
@@ -18202,7 +18214,7 @@
       <c r="AG115" s="15"/>
       <c r="AH115" s="15"/>
     </row>
-    <row r="116" spans="1:34" s="5" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:34" s="5" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A116" s="31" t="s">
         <v>757</v>
       </c>
@@ -18292,7 +18304,7 @@
       <c r="AG116" s="15"/>
       <c r="AH116" s="15"/>
     </row>
-    <row r="117" spans="1:34" s="5" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:34" s="5" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A117" s="31" t="s">
         <v>275</v>
       </c>
@@ -18382,7 +18394,7 @@
       <c r="AG117" s="15"/>
       <c r="AH117" s="15"/>
     </row>
-    <row r="118" spans="1:34" s="5" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:34" s="5" customFormat="1" ht="126" x14ac:dyDescent="0.25">
       <c r="A118" s="31" t="s">
         <v>276</v>
       </c>
@@ -18472,7 +18484,7 @@
       <c r="AG118" s="15"/>
       <c r="AH118" s="15"/>
     </row>
-    <row r="119" spans="1:34" s="5" customFormat="1" ht="234" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:34" s="5" customFormat="1" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A119" s="31" t="s">
         <v>277</v>
       </c>
@@ -18562,7 +18574,7 @@
       <c r="AG119" s="15"/>
       <c r="AH119" s="15"/>
     </row>
-    <row r="120" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A120" s="31" t="s">
         <v>278</v>
       </c>
@@ -18652,7 +18664,7 @@
       <c r="AG120" s="15"/>
       <c r="AH120" s="15"/>
     </row>
-    <row r="121" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A121" s="31" t="s">
         <v>665</v>
       </c>
@@ -18742,7 +18754,7 @@
       <c r="AG121" s="15"/>
       <c r="AH121" s="15"/>
     </row>
-    <row r="122" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A122" s="31" t="s">
         <v>279</v>
       </c>
@@ -18832,7 +18844,7 @@
       <c r="AG122" s="15"/>
       <c r="AH122" s="15"/>
     </row>
-    <row r="123" spans="1:34" s="5" customFormat="1" ht="202.8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:34" s="5" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A123" s="31" t="s">
         <v>1245</v>
       </c>
@@ -18922,7 +18934,7 @@
       <c r="AG123" s="15"/>
       <c r="AH123" s="15"/>
     </row>
-    <row r="124" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A124" s="31" t="s">
         <v>281</v>
       </c>
@@ -19012,7 +19024,7 @@
       <c r="AG124" s="15"/>
       <c r="AH124" s="15"/>
     </row>
-    <row r="125" spans="1:34" s="5" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:34" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A125" s="31" t="s">
         <v>282</v>
       </c>
@@ -19062,10 +19074,10 @@
         <v>283</v>
       </c>
       <c r="Q125" s="34" t="s">
-        <v>30</v>
+        <v>1272</v>
       </c>
       <c r="R125" s="34" t="s">
-        <v>30</v>
+        <v>1273</v>
       </c>
       <c r="S125" s="33" t="b">
         <v>0</v>
@@ -19102,7 +19114,7 @@
       <c r="AG125" s="15"/>
       <c r="AH125" s="15"/>
     </row>
-    <row r="126" spans="1:34" s="5" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:34" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A126" s="31" t="s">
         <v>284</v>
       </c>
@@ -19152,7 +19164,7 @@
         <v>58</v>
       </c>
       <c r="Q126" s="34" t="s">
-        <v>30</v>
+        <v>1274</v>
       </c>
       <c r="R126" s="34" t="s">
         <v>30</v>
@@ -19192,7 +19204,7 @@
       <c r="AG126" s="15"/>
       <c r="AH126" s="15"/>
     </row>
-    <row r="127" spans="1:34" s="5" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:34" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A127" s="31" t="s">
         <v>1178</v>
       </c>
@@ -19242,7 +19254,7 @@
         <v>1181</v>
       </c>
       <c r="Q127" s="34" t="s">
-        <v>30</v>
+        <v>1275</v>
       </c>
       <c r="R127" s="34" t="s">
         <v>30</v>
@@ -19282,7 +19294,7 @@
       <c r="AG127" s="15"/>
       <c r="AH127" s="15"/>
     </row>
-    <row r="128" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A128" s="31" t="s">
         <v>285</v>
       </c>
@@ -19372,7 +19384,7 @@
       <c r="AG128" s="15"/>
       <c r="AH128" s="15"/>
     </row>
-    <row r="129" spans="1:34" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:34" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A129" s="31" t="s">
         <v>286</v>
       </c>
@@ -19462,7 +19474,7 @@
       <c r="AG129" s="15"/>
       <c r="AH129" s="15"/>
     </row>
-    <row r="130" spans="1:34" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:34" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A130" s="31" t="s">
         <v>287</v>
       </c>
@@ -19552,7 +19564,7 @@
       <c r="AG130" s="15"/>
       <c r="AH130" s="15"/>
     </row>
-    <row r="131" spans="1:34" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:34" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="31" t="s">
         <v>758</v>
       </c>
@@ -19644,7 +19656,7 @@
       <c r="AG131" s="15"/>
       <c r="AH131" s="15"/>
     </row>
-    <row r="132" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A132" s="37" t="s">
         <v>756</v>
       </c>
@@ -19734,7 +19746,7 @@
       <c r="AG132" s="15"/>
       <c r="AH132" s="15"/>
     </row>
-    <row r="133" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A133" s="37" t="s">
         <v>755</v>
       </c>
@@ -19824,7 +19836,7 @@
       <c r="AG133" s="15"/>
       <c r="AH133" s="15"/>
     </row>
-    <row r="134" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A134" s="37" t="s">
         <v>754</v>
       </c>
@@ -19914,7 +19926,7 @@
       <c r="AG134" s="15"/>
       <c r="AH134" s="15"/>
     </row>
-    <row r="135" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A135" s="37" t="s">
         <v>753</v>
       </c>
@@ -20004,7 +20016,7 @@
       <c r="AG135" s="15"/>
       <c r="AH135" s="15"/>
     </row>
-    <row r="136" spans="1:34" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:34" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="37" t="s">
         <v>752</v>
       </c>
@@ -20094,7 +20106,7 @@
       <c r="AG136" s="15"/>
       <c r="AH136" s="15"/>
     </row>
-    <row r="137" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A137" s="31" t="s">
         <v>762</v>
       </c>
@@ -20184,7 +20196,7 @@
       <c r="AG137" s="15"/>
       <c r="AH137" s="15"/>
     </row>
-    <row r="138" spans="1:34" s="5" customFormat="1" ht="218.4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:34" s="5" customFormat="1" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A138" s="31" t="s">
         <v>1099</v>
       </c>
@@ -20274,7 +20286,7 @@
       <c r="AG138" s="15"/>
       <c r="AH138" s="15"/>
     </row>
-    <row r="139" spans="1:34" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:34" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A139" s="31" t="s">
         <v>209</v>
       </c>
@@ -20364,7 +20376,7 @@
       <c r="AG139" s="15"/>
       <c r="AH139" s="15"/>
     </row>
-    <row r="140" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:34" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A140" s="34" t="s">
         <v>750</v>
       </c>
@@ -20454,7 +20466,7 @@
       <c r="AG140" s="15"/>
       <c r="AH140" s="15"/>
     </row>
-    <row r="141" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A141" s="34" t="s">
         <v>751</v>
       </c>
@@ -20544,7 +20556,7 @@
       <c r="AG141" s="15"/>
       <c r="AH141" s="15"/>
     </row>
-    <row r="142" spans="1:34" s="5" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:34" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A142" s="34" t="s">
         <v>195</v>
       </c>
@@ -20634,7 +20646,7 @@
       <c r="AG142" s="15"/>
       <c r="AH142" s="15"/>
     </row>
-    <row r="143" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A143" s="37" t="s">
         <v>231</v>
       </c>
@@ -20724,7 +20736,7 @@
       <c r="AG143" s="15"/>
       <c r="AH143" s="15"/>
     </row>
-    <row r="144" spans="1:34" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:34" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A144" s="31" t="s">
         <v>744</v>
       </c>
@@ -20814,7 +20826,7 @@
       <c r="AG144" s="15"/>
       <c r="AH144" s="15"/>
     </row>
-    <row r="145" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A145" s="31" t="s">
         <v>235</v>
       </c>
@@ -20904,7 +20916,7 @@
       <c r="AG145" s="15"/>
       <c r="AH145" s="15"/>
     </row>
-    <row r="146" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A146" s="31" t="s">
         <v>239</v>
       </c>
@@ -20994,7 +21006,7 @@
       <c r="AG146" s="15"/>
       <c r="AH146" s="15"/>
     </row>
-    <row r="147" spans="1:34" s="5" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:34" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A147" s="31" t="s">
         <v>200</v>
       </c>
@@ -21084,7 +21096,7 @@
       <c r="AG147" s="15"/>
       <c r="AH147" s="15"/>
     </row>
-    <row r="148" spans="1:34" s="5" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:34" s="5" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A148" s="31" t="s">
         <v>206</v>
       </c>
@@ -21174,7 +21186,7 @@
       <c r="AG148" s="15"/>
       <c r="AH148" s="15"/>
     </row>
-    <row r="149" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A149" s="37" t="s">
         <v>243</v>
       </c>
@@ -21264,7 +21276,7 @@
       <c r="AG149" s="15"/>
       <c r="AH149" s="15"/>
     </row>
-    <row r="150" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A150" s="37" t="s">
         <v>246</v>
       </c>
@@ -21354,7 +21366,7 @@
       <c r="AG150" s="15"/>
       <c r="AH150" s="15"/>
     </row>
-    <row r="151" spans="1:34" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:34" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A151" s="34" t="s">
         <v>214</v>
       </c>
@@ -21444,7 +21456,7 @@
       <c r="AG151" s="15"/>
       <c r="AH151" s="15"/>
     </row>
-    <row r="152" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A152" s="34" t="s">
         <v>249</v>
       </c>
@@ -21534,7 +21546,7 @@
       <c r="AG152" s="15"/>
       <c r="AH152" s="15"/>
     </row>
-    <row r="153" spans="1:34" s="5" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:34" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A153" s="31" t="s">
         <v>1098</v>
       </c>
@@ -21624,7 +21636,7 @@
       <c r="AG153" s="15"/>
       <c r="AH153" s="15"/>
     </row>
-    <row r="154" spans="1:34" s="5" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:34" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A154" s="31" t="s">
         <v>1097</v>
       </c>
@@ -21714,7 +21726,7 @@
       <c r="AG154" s="15"/>
       <c r="AH154" s="15"/>
     </row>
-    <row r="155" spans="1:34" s="5" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:34" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A155" s="31" t="s">
         <v>1194</v>
       </c>
@@ -21804,7 +21816,7 @@
       <c r="AG155" s="15"/>
       <c r="AH155" s="15"/>
     </row>
-    <row r="156" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A156" s="31" t="s">
         <v>1193</v>
       </c>
@@ -21894,7 +21906,7 @@
       <c r="AG156" s="15"/>
       <c r="AH156" s="15"/>
     </row>
-    <row r="157" spans="1:34" s="5" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:34" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A157" s="31" t="s">
         <v>1224</v>
       </c>
@@ -21984,7 +21996,7 @@
       <c r="AG157" s="15"/>
       <c r="AH157" s="15"/>
     </row>
-    <row r="158" spans="1:34" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:34" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A158" s="31" t="s">
         <v>1102</v>
       </c>
@@ -22074,7 +22086,7 @@
       <c r="AG158" s="15"/>
       <c r="AH158" s="15"/>
     </row>
-    <row r="159" spans="1:34" s="5" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:34" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A159" s="31" t="s">
         <v>1221</v>
       </c>
@@ -22164,7 +22176,7 @@
       <c r="AG159" s="15"/>
       <c r="AH159" s="15"/>
     </row>
-    <row r="160" spans="1:34" s="5" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:34" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A160" s="31" t="s">
         <v>1100</v>
       </c>

</xml_diff>